<commit_message>
Upload Y4_B2526_Excuses.xlsx via attendance app
</commit_message>
<xml_diff>
--- a/log_history/Y4_B2526_Excuses.xlsx
+++ b/log_history/Y4_B2526_Excuses.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Excuses" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Excuses" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -448,7 +448,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="12" customWidth="1" min="1" max="1"/>
-    <col width="13" customWidth="1" min="2" max="2"/>
+    <col width="17" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
     <col width="10" customWidth="1" min="4" max="4"/>
     <col width="8" customWidth="1" min="5" max="5"/>
@@ -490,22 +490,22 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>210809</t>
+          <t>202089</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>immuno&amp;hema</t>
+          <t>general surgery</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>06/10/2025</t>
+          <t>02/11/2025</t>
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>10:00:00</t>
+          <t>10:30:00</t>
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">

</xml_diff>